<commit_message>
many changes -- too long since last commit.  finished ls model
</commit_message>
<xml_diff>
--- a/Export/Clean_Actions_Report_Modeling.xlsx
+++ b/Export/Clean_Actions_Report_Modeling.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdc4f9836624c718/Documents/Grad-School-Docs/CapstoneProject/Repo/Export/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_CAEA5FD297D9AEEF0C07D3531DAD7C3761B43D3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1031AD1F-A4D5-4C79-828B-9449D23CE272}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>DF</t>
   </si>
@@ -31,26 +37,47 @@
     <t>CompleteDF</t>
   </si>
   <si>
+    <t>LR_Final_ModelingDF</t>
+  </si>
+  <si>
+    <t>RF_Final_ModelingDF</t>
+  </si>
+  <si>
     <t>Drop gsubind (Only kept to inform Imputing).</t>
   </si>
   <si>
     <t>Drop Features with less than 0.05 corr while making sure to have 1 feature per source</t>
   </si>
   <si>
+    <t>Drop features w/ low impDecrease from Round 2</t>
+  </si>
+  <si>
     <t>['gsubind']</t>
   </si>
   <si>
     <t>['exesign', 'aoloch_std', 'bkvlps', 'bkvlps_std', 'caps_std', 'chech', 'ci_std', 'cibegni_std', 'cshpri_std', 'dcpstk', 'defrev', 'defrev_std', 'dvc', 'dvt', 'epsfi', 'epsfi_std', 'epsfx', 'epsfx_std', 'epspi', 'epspi_std', 'esopct', 'esopct_std', 'esubc', 'esubc_std', 'fincf_std', 'fopo', 'gdwl', 'gdwl_std', 'intan', 'intan_std', 'mii', 'mii_std', 'msa', 'msa_std', 'ni_std', 'nopi_std', 'oancf_std', 'opeps', 'opeps_std', 'pnca', 'prca', 'prca_std', 'pstk', 'pstk_std', 're_std', 'rect', 'sppiv', 'sppiv_std', 'tot_tax', 'xint', 'xint_std', 'st_prc_end', 'st_per_lowToStart', 'sec_ajexm', 'sec_trfm_mean', 'sec_trfm_std']</t>
   </si>
   <si>
-    <t>(348, 163)</t>
+    <t>['at', 'lse', 'pi_std', 'rest_count_of_diffs', 'sstk_std', 'xsga']</t>
+  </si>
+  <si>
+    <t>['rat_spcsrc']</t>
+  </si>
+  <si>
+    <t>(348, 161)</t>
+  </si>
+  <si>
+    <t>(347, 23)</t>
+  </si>
+  <si>
+    <t>(347, 28)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +140,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -159,7 +194,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,9 +226,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,6 +278,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,14 +471,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -429,16 +508,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -446,13 +525,47 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>